<commit_message>
More graphs related to model runs.
</commit_message>
<xml_diff>
--- a/general/floor_area.xlsx
+++ b/general/floor_area.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,31 +112,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -148,81 +138,37 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,255 +463,337 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33.17" customWidth="1"/>
-    <col min="2" max="2" width="12.24" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1725</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>1745</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1912</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1736</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>1445</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>1672</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+      <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="C30">
         <v>2068</v>
       </c>
     </row>

</xml_diff>